<commit_message>
Added expected output for 18th test case
</commit_message>
<xml_diff>
--- a/Middle Assignment 1/Middle Assignment 1.xlsx
+++ b/Middle Assignment 1/Middle Assignment 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\Middle Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC17FF9-B559-4C83-83D7-7E5DB59A594B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A22836-BDBE-4207-824A-F70701833E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,11 +151,11 @@
     <t>Verify the correct alignment of the price and product name</t>
   </si>
   <si>
-    <t>Verify that the &lt;&gt; button can help users navigate between photos</t>
+    <t xml:space="preserve"> - Case 1: The &lt; button can help users navigate to the previous photo
+- Case 2: The &gt; button can help users navigate to the next photo</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Case 1: The &lt; button can help users navigate to the previous photo
-- Case 2: The &gt; button can help users navigate to the next photo</t>
+    <t>Verify that the &lt;&gt; button can help users navigate between photo</t>
   </si>
 </sst>
 </file>
@@ -351,6 +351,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,21 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,16 +599,16 @@
   </sheetPr>
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7265625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" style="17" customWidth="1"/>
     <col min="3" max="3" width="24.08984375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" style="14" customWidth="1"/>
     <col min="5" max="9" width="12.6328125" style="12"/>
   </cols>
   <sheetData>
@@ -659,17 +659,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -689,17 +689,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -722,7 +722,7 @@
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4"/>
@@ -755,7 +755,7 @@
         <f t="shared" ref="A5:A12" ca="1" si="0">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4"/>
@@ -788,7 +788,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4"/>
@@ -821,7 +821,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="4"/>
@@ -854,7 +854,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="4"/>
@@ -887,7 +887,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="4"/>
@@ -916,17 +916,17 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -949,7 +949,7 @@
       <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="4"/>
@@ -982,7 +982,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="4"/>
@@ -1011,17 +1011,17 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1041,17 +1041,17 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1074,7 +1074,7 @@
       <c r="A15" s="7">
         <v>9</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="4"/>
@@ -1090,7 +1090,7 @@
         <f t="shared" ref="A16:A22" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
         <v>10</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4"/>
@@ -1106,7 +1106,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="4"/>
@@ -1122,7 +1122,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="4"/>
@@ -1137,7 +1137,7 @@
       <c r="A19" s="9">
         <v>16</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="4"/>
@@ -1153,7 +1153,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>17</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="4"/>
@@ -1169,7 +1169,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="4"/>
@@ -1185,7 +1185,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="4"/>
@@ -1197,17 +1197,17 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1230,16 +1230,16 @@
       <c r="A24" s="13">
         <v>18</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="22"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="27" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="22"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
-      <c r="B28" s="22"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="29" spans="1:26" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
-      <c r="B29" s="22"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="22"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="31" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="22"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="32" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="22"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="33" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="22"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>

</xml_diff>